<commit_message>
updated TC001CreateGoodReceipt and TestActionLibrary
</commit_message>
<xml_diff>
--- a/SystemTest/SmokeSanityExecutionResult_LPH_V1.9.0.xlsx
+++ b/SystemTest/SmokeSanityExecutionResult_LPH_V1.9.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23265" yWindow="0" windowWidth="13905" windowHeight="12300"/>
+    <workbookView xWindow="24210" yWindow="0" windowWidth="13905" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -57,96 +57,114 @@
     <t>Patient\TC001PatientRegistrationPrintHealthCard.py</t>
   </si>
   <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>OnHold</t>
+  </si>
+  <si>
+    <t>Billing\Opbilling\TC002OPDbillingLabXray.py</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Laboratory\TC005GenerateLabReport.py</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>Radiology\TC001GenerateUSGReport.py</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>Pharmacy\TC003PharmacyOPDbilling.py</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\TC010VerifyPharmacyDashboard.py</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ADT\TC009AdmissionDischargeTransferToBeRefund.py</t>
+  </si>
+  <si>
+    <t>SanityTest</t>
+  </si>
+  <si>
+    <t>TC008</t>
+  </si>
+  <si>
+    <t>ADT\TC011AdmissionDischargeTransferNoDeposit.py</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>Nursing\TC001WardBilling&amp;AddVitals.py</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>Appointment\TC002CreateAppointmentFollowup.py</t>
+  </si>
+  <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>TC002</t>
-  </si>
-  <si>
-    <t>Billing\Opbilling\TC002OPDbillingLabXray.py</t>
-  </si>
-  <si>
-    <t>TC003</t>
-  </si>
-  <si>
-    <t>Laboratory\TC005GenerateLabReport.py</t>
-  </si>
-  <si>
-    <t>TC004</t>
-  </si>
-  <si>
-    <t>Radiology\TC001GenerateUSGReport.py</t>
-  </si>
-  <si>
-    <t>TC005</t>
-  </si>
-  <si>
-    <t>Pharmacy\TC003PharmacyOPDbilling.py</t>
-  </si>
-  <si>
-    <t>TC006</t>
-  </si>
-  <si>
-    <t>Pharmacy\Reports\TC010VerifyPharmacyDashboard.py</t>
-  </si>
-  <si>
-    <t>TC007</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>ADT\TC009AdmissionDischargeTransferToBeRefund.py</t>
-  </si>
-  <si>
-    <t>SanityTest</t>
-  </si>
-  <si>
-    <t>TC008</t>
-  </si>
-  <si>
-    <t>ADT\TC011AdmissionDischargeTransferNoDeposit.py</t>
-  </si>
-  <si>
-    <t>TC009</t>
-  </si>
-  <si>
-    <t>Nursing\TC001WardBilling&amp;AddVitals.py</t>
-  </si>
-  <si>
-    <t>TC010</t>
-  </si>
-  <si>
-    <t>Appointment\TC002CreateAppointmentFollowup.py</t>
-  </si>
-  <si>
     <t>TC011</t>
   </si>
   <si>
+    <t>M &amp; S</t>
+  </si>
+  <si>
     <t>Reports\TC001BillingDashboardSummary.py</t>
   </si>
   <si>
     <t>TC012</t>
   </si>
   <si>
+    <t>LPH-864</t>
+  </si>
+  <si>
     <t>Billing\OPbilling\TC012CreateCopyOfItemsCreditInvoice.py</t>
   </si>
   <si>
     <t>TC013</t>
   </si>
   <si>
+    <t>LPH-865</t>
+  </si>
+  <si>
     <t>Reports\TC003SalesDayBookReport.py</t>
   </si>
   <si>
     <t>TC014</t>
   </si>
   <si>
+    <t>Report Hide</t>
+  </si>
+  <si>
     <t>Reports\TC005IncomeSegregationReport.py</t>
   </si>
   <si>
     <t>TC016</t>
   </si>
   <si>
+    <t>LPH-866</t>
+  </si>
+  <si>
     <t>Reports\TC006PatientCreditSummaryReport.py</t>
   </si>
   <si>
@@ -165,32 +183,14 @@
     <t>TC019</t>
   </si>
   <si>
-    <t>M &amp; S</t>
-  </si>
-  <si>
-    <t>LPH-864</t>
-  </si>
-  <si>
-    <t>LPH-865</t>
-  </si>
-  <si>
-    <t>Report Hide</t>
-  </si>
-  <si>
-    <t>LPH-866</t>
-  </si>
-  <si>
     <t>LPH-867</t>
-  </si>
-  <si>
-    <t>OnHold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +232,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -308,17 +316,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FF00FF00"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -596,7 +600,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,8 +658,8 @@
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
@@ -664,11 +668,11 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="6" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -694,8 +698,8 @@
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -715,8 +719,8 @@
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
@@ -736,8 +740,8 @@
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
@@ -757,8 +761,8 @@
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
@@ -781,8 +785,8 @@
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>26</v>
@@ -802,14 +806,14 @@
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>29</v>
@@ -842,119 +846,119 @@
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
+      <c r="B12" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="7" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>12</v>
+        <v>48</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>26</v>
@@ -963,55 +967,53 @@
         <v>2</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>12</v>
+        <v>50</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated TC and TestActionLibrary for LPH_V1.9.1
</commit_message>
<xml_diff>
--- a/SystemTest/SmokeSanityExecutionResult_LPH_V1.9.0.xlsx
+++ b/SystemTest/SmokeSanityExecutionResult_LPH_V1.9.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24210" yWindow="0" windowWidth="13905" windowHeight="12300"/>
+    <workbookView xWindow="25155" yWindow="0" windowWidth="13905" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -600,7 +600,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>